<commit_message>
envio de arquivos da aula 6
</commit_message>
<xml_diff>
--- a/Aula06_DispersaoAssociacao/Mundo.xlsx
+++ b/Aula06_DispersaoAssociacao/Mundo.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="12120" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="mundo" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="SPSS">mundo!$B$1:$J$86</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="80000"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>X1</t>
   </si>
@@ -52,26 +51,11 @@
   <si>
     <t>i</t>
   </si>
-  <si>
-    <t>Cov(X3,X4)=</t>
-  </si>
-  <si>
-    <t>DP(X3)=</t>
-  </si>
-  <si>
-    <t>Corr(X3,X4)=</t>
-  </si>
-  <si>
-    <t>DP(X4)=</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
@@ -118,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -141,10 +125,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N87"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -464,11 +444,11 @@
     <col min="9" max="9" width="8.625" style="1" customWidth="1"/>
     <col min="10" max="10" width="5.625" style="1" customWidth="1"/>
     <col min="11" max="12" width="11.375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="9.125" style="1" customWidth="1"/>
     <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
@@ -503,7 +483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -538,15 +518,8 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="L2" s="4"/>
-      <c r="M2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="10">
-        <f>_xlfn.COVARIANCE.P(D2:D86,E2:E86)</f>
-        <v>192.06339100346023</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -581,15 +554,8 @@
         <v>0.33900000000000002</v>
       </c>
       <c r="L3" s="4"/>
-      <c r="M3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="10">
-        <f>_xlfn.STDEV.P(D2:D86)</f>
-        <v>24.092026563671158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -624,15 +590,8 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="L4" s="4"/>
-      <c r="M4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" s="10">
-        <f>_xlfn.STDEV.P(E2:E86)</f>
-        <v>10.661082736809956</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -668,7 +627,7 @@
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -703,15 +662,8 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="L6" s="4"/>
-      <c r="M6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="N6" s="10">
-        <f>N2/(N3*N4)</f>
-        <v>0.74777328460510428</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -747,7 +699,7 @@
       </c>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -783,7 +735,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -819,7 +771,7 @@
       </c>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -855,7 +807,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -891,7 +843,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -927,7 +879,7 @@
       </c>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -963,7 +915,7 @@
       </c>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -999,7 +951,7 @@
       </c>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -1035,7 +987,7 @@
       </c>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -3600,16 +3552,4 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>